<commit_message>
agregando casos para cada tipo de celda
</commit_message>
<xml_diff>
--- a/leeme.xlsx
+++ b/leeme.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andres\Documents\UNIVERSIDAD\PROYECTO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D204E16B-6593-4632-B1A3-DAA729A16582}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9416261D-3B5F-4EE0-89D0-50E4A90E35B2}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14640" windowHeight="4920" xr2:uid="{018E3A0E-FAD5-4C26-99DB-BB86D26D1348}"/>
   </bookViews>
@@ -24,10 +24,35 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>Maria E</t>
+  </si>
+  <si>
+    <t>Andres</t>
+  </si>
+  <si>
+    <t>Alejandro</t>
+  </si>
+  <si>
+    <t>Esteban</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -55,8 +80,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -371,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72E7A0C5-3765-4DE7-B6B2-26B77AEB2116}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -383,59 +410,63 @@
       <c r="A1">
         <v>1</v>
       </c>
-      <c r="B1">
-        <v>2</v>
-      </c>
-      <c r="C1">
-        <v>3</v>
+      <c r="B1" s="1">
+        <v>36785</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
       </c>
       <c r="D1">
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>8</v>
-      </c>
-      <c r="B2">
-        <v>7</v>
-      </c>
-      <c r="C2">
-        <v>6</v>
+        <v>2</v>
+      </c>
+      <c r="B2" s="1">
+        <v>27523</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>5</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>9</v>
-      </c>
-      <c r="B3">
-        <v>10</v>
-      </c>
-      <c r="C3">
-        <v>11</v>
+        <v>3</v>
+      </c>
+      <c r="B3" s="1">
+        <v>25809</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
       </c>
       <c r="D3">
-        <v>12</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>16</v>
-      </c>
-      <c r="B4">
-        <v>15</v>
-      </c>
-      <c r="C4">
-        <v>14</v>
+        <v>4</v>
+      </c>
+      <c r="B4" s="1">
+        <v>41436</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
       </c>
       <c r="D4">
-        <v>13</v>
-      </c>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
corrigiendo error formato fecha
</commit_message>
<xml_diff>
--- a/leeme.xlsx
+++ b/leeme.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andres\Documents\UNIVERSIDAD\PROYECTO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9416261D-3B5F-4EE0-89D0-50E4A90E35B2}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BFD5D8C-693D-4E5C-BAB4-C3F72914E044}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14640" windowHeight="4920" xr2:uid="{018E3A0E-FAD5-4C26-99DB-BB86D26D1348}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Maria E</t>
   </si>
@@ -37,6 +37,18 @@
   </si>
   <si>
     <t>Esteban</t>
+  </si>
+  <si>
+    <t>16-09-2000</t>
+  </si>
+  <si>
+    <t>09-05-1975</t>
+  </si>
+  <si>
+    <t>28-08-1970</t>
+  </si>
+  <si>
+    <t>11-06-2013</t>
   </si>
 </sst>
 </file>
@@ -80,10 +92,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -401,17 +414,21 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" style="1"/>
+    <col min="2" max="2" width="31.28515625" style="2" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1">
+      <c r="A1" s="1">
         <v>1</v>
       </c>
-      <c r="B1" s="1">
-        <v>36785</v>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -421,11 +438,11 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>2</v>
       </c>
-      <c r="B2" s="1">
-        <v>27523</v>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -435,11 +452,11 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>3</v>
       </c>
-      <c r="B3" s="1">
-        <v>25809</v>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -449,11 +466,11 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>4</v>
       </c>
-      <c r="B4" s="1">
-        <v>41436</v>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -463,7 +480,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="2"/>
+      <c r="B5" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>